<commit_message>
final version of catalog
</commit_message>
<xml_diff>
--- a/Final Project/Final Application/catalog.xlsx
+++ b/Final Project/Final Application/catalog.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$42</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>/Final Application</t>
   </si>
@@ -112,6 +112,36 @@
   </si>
   <si>
     <t>Updated / completed Gantt Chart</t>
+  </si>
+  <si>
+    <t>/src/main/java/fhirwhenready</t>
+  </si>
+  <si>
+    <t>fhir</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>servlet</t>
+  </si>
+  <si>
+    <t>api/dao</t>
+  </si>
+  <si>
+    <t>apiimpl</t>
+  </si>
+  <si>
+    <t>Data Access component from HAPI FHIR</t>
+  </si>
+  <si>
+    <t>Implementation of DAO</t>
+  </si>
+  <si>
+    <t>Classes for data transfer &amp; storage</t>
+  </si>
+  <si>
+    <t>Servlets for HTTP endpoint interfaces</t>
   </si>
 </sst>
 </file>
@@ -534,18 +564,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -697,34 +729,109 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
catalog - added special instructions
</commit_message>
<xml_diff>
--- a/Final Project/Final Application/catalog.xlsx
+++ b/Final Project/Final Application/catalog.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$44</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>/Final Application</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Manual - Team FHIR When Ready.pdf</t>
+  </si>
+  <si>
+    <t>Special Instructions - Team FHIR When Ready.pdf</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,49 +736,44 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>31</v>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
@@ -785,23 +783,24 @@
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="7">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>32</v>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -811,40 +810,53 @@
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <v>2</v>
       </c>
       <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>